<commit_message>
Updated particpant ID list
</commit_message>
<xml_diff>
--- a/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
+++ b/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
@@ -1637,7 +1637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1668,9 +1668,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1976,28 +1973,28 @@
   <dimension ref="A1:AML83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.73046875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="67.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="54.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" style="1" customWidth="1"/>
-    <col min="14" max="1026" width="14.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="67.86328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="34.1328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.73046875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="54.265625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="29.1328125" style="1" customWidth="1"/>
+    <col min="14" max="1026" width="14.1328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1026" s="4" customFormat="1">
@@ -2041,7 +2038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1026" ht="105">
+    <row r="2" spans="1:1026" ht="85.5">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -2060,8 +2057,8 @@
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2">
-        <f>0</f>
+      <c r="G2" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -2080,7 +2077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1026" ht="45">
+    <row r="3" spans="1:1026" ht="42.75">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2099,8 +2096,8 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2">
-        <f>0</f>
+      <c r="G3" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -2116,7 +2113,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:1026" ht="30">
+    <row r="4" spans="1:1026" ht="28.5">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2135,8 +2132,8 @@
       <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="2">
-        <f>0</f>
+      <c r="G4" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -2152,7 +2149,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:1026" ht="135">
+    <row r="5" spans="1:1026" ht="99.75">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2171,8 +2168,8 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2">
-        <f>0</f>
+      <c r="G5" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I5" s="7" t="s">
@@ -2191,7 +2188,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:1026" ht="90">
+    <row r="6" spans="1:1026" ht="71.25">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2210,8 +2207,8 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="2">
-        <f>0</f>
+      <c r="G6" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -2230,7 +2227,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="7" spans="1:1026" ht="30">
+    <row r="7" spans="1:1026" ht="28.5">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -2249,8 +2246,8 @@
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2">
-        <f>0</f>
+      <c r="G7" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -2269,7 +2266,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="8" spans="1:1026" ht="180">
+    <row r="8" spans="1:1026" ht="142.5">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2288,8 +2285,8 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="2">
-        <f>0</f>
+      <c r="G8" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -2302,7 +2299,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:1026" ht="180">
+    <row r="9" spans="1:1026" ht="171">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -2321,8 +2318,8 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="2">
-        <f>0</f>
+      <c r="G9" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -2338,7 +2335,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:1026" ht="195">
+    <row r="10" spans="1:1026" ht="156.75">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -2357,8 +2354,8 @@
       <c r="F10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="2">
-        <f>0</f>
+      <c r="G10" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -2374,7 +2371,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="11" spans="1:1026" s="14" customFormat="1" ht="45">
+    <row r="11" spans="1:1026" s="13" customFormat="1" ht="28.5">
       <c r="A11" s="11" t="s">
         <v>62</v>
       </c>
@@ -2393,19 +2390,19 @@
       <c r="F11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="12">
-        <f>0</f>
+      <c r="G11" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H11" s="11"/>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K11" s="11"/>
-      <c r="L11" s="13"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="11" t="s">
         <v>391</v>
       </c>
@@ -3423,7 +3420,7 @@
       <c r="AMK11" s="11"/>
       <c r="AML11" s="11"/>
     </row>
-    <row r="12" spans="1:1026" s="14" customFormat="1" ht="30">
+    <row r="12" spans="1:1026" s="13" customFormat="1" ht="28.5">
       <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
@@ -3442,19 +3439,19 @@
       <c r="F12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="12">
-        <f>0</f>
+      <c r="G12" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="11"/>
-      <c r="L12" s="13"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="11" t="s">
         <v>393</v>
       </c>
@@ -4472,7 +4469,7 @@
       <c r="AMK12" s="11"/>
       <c r="AML12" s="11"/>
     </row>
-    <row r="13" spans="1:1026" s="14" customFormat="1">
+    <row r="13" spans="1:1026" s="13" customFormat="1">
       <c r="A13" s="11" t="s">
         <v>72</v>
       </c>
@@ -4491,19 +4488,19 @@
       <c r="F13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="12">
-        <f>0</f>
+      <c r="G13" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H13" s="11"/>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="11"/>
-      <c r="L13" s="13"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="11" t="s">
         <v>393</v>
       </c>
@@ -5521,7 +5518,7 @@
       <c r="AMK13" s="11"/>
       <c r="AML13" s="11"/>
     </row>
-    <row r="14" spans="1:1026" ht="165">
+    <row r="14" spans="1:1026" ht="156.75">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -5540,8 +5537,8 @@
       <c r="F14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="2">
-        <f>0</f>
+      <c r="G14" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -5560,7 +5557,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="15" spans="1:1026" ht="150">
+    <row r="15" spans="1:1026" ht="142.5">
       <c r="A15" s="1" t="s">
         <v>345</v>
       </c>
@@ -5596,7 +5593,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="16" spans="1:1026" s="14" customFormat="1">
+    <row r="16" spans="1:1026" s="13" customFormat="1">
       <c r="A16" s="11" t="s">
         <v>84</v>
       </c>
@@ -5615,19 +5612,19 @@
       <c r="F16" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="12">
-        <f>0</f>
+      <c r="G16" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>400</v>
       </c>
       <c r="K16" s="11"/>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="12" t="s">
         <v>404</v>
       </c>
       <c r="M16" s="11"/>
@@ -6645,7 +6642,7 @@
       <c r="AMK16" s="11"/>
       <c r="AML16" s="11"/>
     </row>
-    <row r="17" spans="1:1026" ht="135">
+    <row r="17" spans="1:1026" ht="114">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -6664,8 +6661,8 @@
       <c r="F17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="2">
-        <f>0</f>
+      <c r="G17" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -6684,7 +6681,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="18" spans="1:1026" ht="165">
+    <row r="18" spans="1:1026" ht="156.75">
       <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
@@ -6703,8 +6700,8 @@
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="2">
-        <f>0</f>
+      <c r="G18" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
@@ -6716,14 +6713,14 @@
       <c r="K18" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="14" t="s">
         <v>410</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="1:1026" ht="60">
+    <row r="19" spans="1:1026" ht="57">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -6742,8 +6739,8 @@
       <c r="F19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="2">
-        <f>0</f>
+      <c r="G19" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -6759,7 +6756,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="20" spans="1:1026" s="14" customFormat="1" ht="45">
+    <row r="20" spans="1:1026" s="13" customFormat="1" ht="42.75">
       <c r="A20" s="11" t="s">
         <v>104</v>
       </c>
@@ -6778,19 +6775,19 @@
       <c r="F20" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="12">
-        <f>0</f>
+      <c r="G20" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K20" s="11"/>
-      <c r="L20" s="13" t="s">
+      <c r="L20" s="12" t="s">
         <v>413</v>
       </c>
       <c r="M20" s="11"/>
@@ -7808,7 +7805,7 @@
       <c r="AMK20" s="11"/>
       <c r="AML20" s="11"/>
     </row>
-    <row r="21" spans="1:1026" ht="75">
+    <row r="21" spans="1:1026" ht="71.25">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -7827,8 +7824,8 @@
       <c r="F21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="2">
-        <f>0</f>
+      <c r="G21" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I21" s="3" t="s">
@@ -7844,7 +7841,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="22" spans="1:1026" ht="90">
+    <row r="22" spans="1:1026" ht="85.5">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -7863,8 +7860,8 @@
       <c r="F22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="2">
-        <f>0</f>
+      <c r="G22" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -7877,7 +7874,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:1026" ht="30">
+    <row r="23" spans="1:1026" ht="28.5">
       <c r="A23" s="1" t="s">
         <v>351</v>
       </c>
@@ -7943,7 +7940,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:1026" ht="75">
+    <row r="25" spans="1:1026" ht="71.25">
       <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
@@ -7979,7 +7976,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="26" spans="1:1026" ht="30">
+    <row r="26" spans="1:1026" ht="28.5">
       <c r="A26" s="1" t="s">
         <v>433</v>
       </c>
@@ -8016,7 +8013,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="27" spans="1:1026" ht="45">
+    <row r="27" spans="1:1026" ht="42.75">
       <c r="A27" s="1" t="s">
         <v>435</v>
       </c>
@@ -8053,7 +8050,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="28" spans="1:1026" s="14" customFormat="1" ht="30">
+    <row r="28" spans="1:1026" s="13" customFormat="1">
       <c r="A28" s="11" t="s">
         <v>126</v>
       </c>
@@ -8072,19 +8069,19 @@
       <c r="F28" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="12">
-        <f>0</f>
+      <c r="G28" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H28" s="11"/>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K28" s="11"/>
-      <c r="L28" s="13"/>
+      <c r="L28" s="12"/>
       <c r="M28" s="11" t="s">
         <v>426</v>
       </c>
@@ -9102,7 +9099,7 @@
       <c r="AMK28" s="11"/>
       <c r="AML28" s="11"/>
     </row>
-    <row r="29" spans="1:1026" ht="30">
+    <row r="29" spans="1:1026" ht="28.5">
       <c r="A29" s="1" t="s">
         <v>130</v>
       </c>
@@ -9121,15 +9118,15 @@
       <c r="F29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="2">
-        <f>0</f>
+      <c r="G29" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:1026" ht="30">
+    <row r="30" spans="1:1026" ht="28.5">
       <c r="A30" s="1" t="s">
         <v>134</v>
       </c>
@@ -9148,8 +9145,8 @@
       <c r="F30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="2">
-        <f>0</f>
+      <c r="G30" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K30" s="1" t="s">
@@ -9175,8 +9172,8 @@
       <c r="F31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="2">
-        <f>0</f>
+      <c r="G31" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -9199,15 +9196,15 @@
       <c r="F32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="2">
-        <f>0</f>
+      <c r="G32" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="75">
+    <row r="33" spans="1:13" ht="71.25">
       <c r="A33" s="1" t="s">
         <v>145</v>
       </c>
@@ -9226,8 +9223,8 @@
       <c r="F33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="2">
-        <f>0</f>
+      <c r="G33" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K33" s="1" t="s">
@@ -9237,7 +9234,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>148</v>
       </c>
@@ -9256,12 +9253,12 @@
       <c r="F34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="2">
-        <f>0</f>
+      <c r="G34" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="30">
+    <row r="35" spans="1:13" ht="28.5">
       <c r="A35" s="1" t="s">
         <v>151</v>
       </c>
@@ -9280,8 +9277,8 @@
       <c r="F35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="2">
-        <f>1</f>
+      <c r="G35" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -9307,15 +9304,15 @@
       <c r="F36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="2">
-        <f>0</f>
+      <c r="G36" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="30">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>159</v>
       </c>
@@ -9332,8 +9329,8 @@
       <c r="F37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="2">
-        <f>1</f>
+      <c r="G37" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -9343,7 +9340,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="30">
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>163</v>
       </c>
@@ -9362,12 +9359,12 @@
       <c r="F38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="2">
-        <f>0</f>
+      <c r="G38" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="30">
+    <row r="39" spans="1:13" ht="28.5">
       <c r="A39" s="1" t="s">
         <v>166</v>
       </c>
@@ -9383,15 +9380,15 @@
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="2">
-        <f>0</f>
+      <c r="G39" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="30">
+    <row r="40" spans="1:13" ht="28.5">
       <c r="A40" s="1" t="s">
         <v>172</v>
       </c>
@@ -9408,12 +9405,12 @@
       <c r="F40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="2">
-        <f>0</f>
+      <c r="G40" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="30">
+    <row r="41" spans="1:13" ht="28.5">
       <c r="A41" s="1" t="s">
         <v>175</v>
       </c>
@@ -9429,8 +9426,8 @@
       <c r="F41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="2">
-        <f>1</f>
+      <c r="G41" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -9453,8 +9450,8 @@
       <c r="F42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="2">
-        <f>1</f>
+      <c r="G42" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -9464,7 +9461,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="45">
+    <row r="43" spans="1:13" ht="42.75">
       <c r="A43" s="1" t="s">
         <v>184</v>
       </c>
@@ -9483,8 +9480,8 @@
       <c r="F43" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G43" s="2">
-        <f>0</f>
+      <c r="G43" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9505,15 +9502,15 @@
       <c r="F44" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G44" s="2">
-        <f>0</f>
+      <c r="G44" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="30">
+    <row r="45" spans="1:13" ht="28.5">
       <c r="A45" s="1" t="s">
         <v>191</v>
       </c>
@@ -9532,12 +9529,12 @@
       <c r="F45" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G45" s="2">
-        <f>0</f>
+      <c r="G45" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="30">
+    <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
         <v>194</v>
       </c>
@@ -9581,8 +9578,8 @@
       <c r="F47" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G47" s="2">
-        <f>0</f>
+      <c r="G47" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9603,8 +9600,8 @@
       <c r="F48" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G48" s="2">
-        <f>0</f>
+      <c r="G48" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9625,8 +9622,8 @@
       <c r="F49" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G49" s="2">
-        <f>0</f>
+      <c r="G49" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9647,8 +9644,8 @@
       <c r="F50" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G50" s="2">
-        <f>0</f>
+      <c r="G50" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9669,8 +9666,8 @@
       <c r="F51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G51" s="2">
-        <f>0</f>
+      <c r="G51" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9691,8 +9688,8 @@
       <c r="F52" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G52" s="2">
-        <f>0</f>
+      <c r="G52" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9712,8 +9709,8 @@
       <c r="F53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G53" s="2">
-        <f>0</f>
+      <c r="G53" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9734,8 +9731,8 @@
       <c r="F54" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G54" s="2">
-        <f>0</f>
+      <c r="G54" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9756,8 +9753,8 @@
       <c r="F55" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G55" s="2">
-        <f>0</f>
+      <c r="G55" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9778,8 +9775,8 @@
       <c r="F56" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G56" s="2">
-        <f>0</f>
+      <c r="G56" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9800,8 +9797,8 @@
       <c r="F57" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G57" s="2">
-        <f>0</f>
+      <c r="G57" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9822,8 +9819,8 @@
       <c r="F58" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G58" s="2">
-        <f>0</f>
+      <c r="G58" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9844,8 +9841,8 @@
       <c r="F59" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G59" s="2">
-        <f>0</f>
+      <c r="G59" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9866,8 +9863,8 @@
       <c r="F60" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G60" s="2">
-        <f>0</f>
+      <c r="G60" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9888,8 +9885,8 @@
       <c r="F61" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G61" s="2">
-        <f>0</f>
+      <c r="G61" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9910,8 +9907,8 @@
       <c r="F62" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G62" s="2">
-        <f>0</f>
+      <c r="G62" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9932,8 +9929,8 @@
       <c r="F63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G63" s="2">
-        <f>0</f>
+      <c r="G63" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9954,8 +9951,8 @@
       <c r="F64" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G64" s="2">
-        <f>0</f>
+      <c r="G64" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9976,8 +9973,8 @@
       <c r="F65" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G65" s="2">
-        <f>0</f>
+      <c r="G65" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9998,12 +9995,12 @@
       <c r="F66" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G66" s="2">
-        <f>0</f>
+      <c r="G66" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="30">
+    <row r="67" spans="1:13" ht="28.5">
       <c r="A67" s="9" t="s">
         <v>273</v>
       </c>
@@ -10020,8 +10017,8 @@
       <c r="F67" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G67" s="2">
-        <f>0</f>
+      <c r="G67" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10042,8 +10039,8 @@
       <c r="F68" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G68" s="2">
-        <f>0</f>
+      <c r="G68" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10064,8 +10061,8 @@
       <c r="F69" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G69" s="2">
-        <f>0</f>
+      <c r="G69" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10086,8 +10083,8 @@
       <c r="F70" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G70" s="2">
-        <f>0</f>
+      <c r="G70" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10108,8 +10105,8 @@
       <c r="F71" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G71" s="2">
-        <f>0</f>
+      <c r="G71" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10130,8 +10127,8 @@
       <c r="F72" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G72" s="2">
-        <f>0</f>
+      <c r="G72" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10152,8 +10149,8 @@
       <c r="F73" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G73" s="2">
-        <f>0</f>
+      <c r="G73" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10174,8 +10171,8 @@
       <c r="F74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G74" s="2">
-        <f>0</f>
+      <c r="G74" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10196,8 +10193,8 @@
       <c r="F75" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G75" s="2">
-        <f>0</f>
+      <c r="G75" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10217,8 +10214,8 @@
       <c r="F76" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G76" s="2">
-        <f>0</f>
+      <c r="G76" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10239,12 +10236,12 @@
       <c r="F77" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G77" s="2">
-        <f>0</f>
+      <c r="G77" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="30">
+    <row r="78" spans="1:13">
       <c r="A78" s="9" t="s">
         <v>316</v>
       </c>
@@ -10261,8 +10258,8 @@
       <c r="F78" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="2">
-        <f>0</f>
+      <c r="G78" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10282,8 +10279,8 @@
       <c r="F79" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="G79" s="2">
-        <f>1</f>
+      <c r="G79" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H79" s="1" t="s">
@@ -10309,12 +10306,12 @@
       <c r="F80" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="G80" s="2">
-        <f>0</f>
+      <c r="G80" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="30">
+    <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
         <v>329</v>
       </c>
@@ -10333,8 +10330,8 @@
       <c r="F81" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G81" s="2">
-        <f>0</f>
+      <c r="G81" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I81" s="3" t="s">
@@ -10357,12 +10354,12 @@
       <c r="F82" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G82" s="2">
-        <f>0</f>
+      <c r="G82" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="30">
+    <row r="83" spans="1:13" ht="28.5">
       <c r="A83" s="1" t="s">
         <v>337</v>
       </c>

</xml_diff>